<commit_message>
Paphyrus - 할인율 설정 50%
</commit_message>
<xml_diff>
--- a/resource/Paphyrus/관리자/3. 관리자_지종설정.xlsx
+++ b/resource/Paphyrus/관리자/3. 관리자_지종설정.xlsx
@@ -1313,7 +1313,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1324,8 +1324,8 @@
   <dimension ref="A1:I1091"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1003" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1018" sqref="G1018"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -25341,5 +25341,6 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>